<commit_message>
In order to calibrate, program was given y and sensed x. To get the desired transfer function, needed to inverse the function output.
</commit_message>
<xml_diff>
--- a/Calibration_Values.xlsx
+++ b/Calibration_Values.xlsx
@@ -1,88 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cooper.hanley\Desktop\Linear_Calibration\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACFEB37-5D37-4586-B319-099A15A0E60B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="435" windowWidth="21600" windowHeight="14175" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>xValue</t>
-  </si>
-  <si>
-    <t>sensorValue</t>
-  </si>
-  <si>
-    <t>STD</t>
-  </si>
-  <si>
-    <t>Slope</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Y-int</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>3000</t>
-  </si>
-  <si>
-    <t>4000</t>
-  </si>
-  <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>6000</t>
-  </si>
-  <si>
-    <t>7000</t>
-  </si>
-  <si>
-    <t>8000</t>
-  </si>
-  <si>
-    <t>9000</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -101,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -415,151 +419,185 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col width="6.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="12" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="6.7109375" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>1.2649782379594719E-4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>0.47889152702689169</v>
-      </c>
-      <c r="C2">
-        <v>1.2809682025626131E-4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>0.47167563256946432</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>0.59559115105867388</v>
-      </c>
-      <c r="C3">
-        <v>1.1781022425145031E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>yValue</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sensorValue</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>STD</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Slope</t>
+        </is>
+      </c>
+      <c r="F1" t="n">
+        <v>7904.438376224025</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.4788915270268917</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0001280968202562613</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Y-int</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>-3727.855109358608</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5955911510586739</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.01178102242514503</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>0.7211763015389443</v>
       </c>
-      <c r="C4">
-        <v>2.0530697319850209E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>0.84809126836061477</v>
-      </c>
-      <c r="C5">
-        <v>2.5805098716312289E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>0.97607331228256222</v>
-      </c>
-      <c r="C6">
-        <v>3.8251689746732598E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>1.1020754336118701</v>
-      </c>
-      <c r="C7">
-        <v>2.8359669761594038E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>1.2311129492521291</v>
-      </c>
-      <c r="C8">
-        <v>3.0373931407896359E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>1.3642248353958131</v>
-      </c>
-      <c r="C9">
-        <v>3.2566723522443337E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>1.4831508340835571</v>
-      </c>
-      <c r="C10">
-        <v>3.4672006179807757E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>1.6087707839012151</v>
-      </c>
-      <c r="C11">
-        <v>3.3223888532490267E-2</v>
+      <c r="C4" t="n">
+        <v>0.02053069731985021</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.8480912683606148</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.02580509871631229</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>4000</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.9760733122825622</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0382516897467326</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1.10207543361187</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.02835966976159404</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.231112949252129</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.03037393140789636</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>7000</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1.364224835395813</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.03256672352244334</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1.483150834083557</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.03467200617980776</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>9000</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1.608770783901215</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.03322388853249027</v>
       </c>
     </row>
   </sheetData>

</xml_diff>